<commit_message>
SVR parameter calc CRPS
</commit_message>
<xml_diff>
--- a/thesis work/code and more/models/SVR kernel and parameter scores.xlsx
+++ b/thesis work/code and more/models/SVR kernel and parameter scores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Uni\Bachelorarbeit\code\BachelorThesisWPF\thesis work\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Uni\Bachelorarbeit\code\BachelorThesisWPF\thesis work\code and more\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC662CC-B108-47E7-A9F6-48B7D82ABE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093E2739-B314-4B0B-9F95-1FA2E3760FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>SVR</t>
-  </si>
-  <si>
-    <t>Model Nr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t>Kernel</t>
   </si>
@@ -52,6 +46,234 @@
   </si>
   <si>
     <t>CRPS</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>77.70</t>
+  </si>
+  <si>
+    <t>125.46</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>127.60</t>
+  </si>
+  <si>
+    <t>49.73</t>
+  </si>
+  <si>
+    <t>81.99</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>124.08</t>
+  </si>
+  <si>
+    <t>233.40</t>
+  </si>
+  <si>
+    <t>433.52</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>96.58</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>45.92</t>
+  </si>
+  <si>
+    <t>74.60</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>123.41</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>42.75</t>
+  </si>
+  <si>
+    <t>68.80</t>
+  </si>
+  <si>
+    <t>122.83</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>41.18</t>
+  </si>
+  <si>
+    <t>64.01</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>122.62</t>
+  </si>
+  <si>
+    <t>40.34</t>
+  </si>
+  <si>
+    <t>62.02</t>
+  </si>
+  <si>
+    <t>122.44</t>
+  </si>
+  <si>
+    <t>250.0</t>
+  </si>
+  <si>
+    <t>41.32</t>
+  </si>
+  <si>
+    <t>61.33</t>
+  </si>
+  <si>
+    <t>123.26</t>
+  </si>
+  <si>
+    <t>48.43</t>
+  </si>
+  <si>
+    <t>65.70</t>
+  </si>
+  <si>
+    <t>350.0</t>
+  </si>
+  <si>
+    <t>131.38</t>
+  </si>
+  <si>
+    <t>175.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>40.44</t>
+  </si>
+  <si>
+    <t>61.55</t>
+  </si>
+  <si>
+    <t>122.55</t>
+  </si>
+  <si>
+    <t>180.0</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>40.85</t>
+  </si>
+  <si>
+    <t>61.70</t>
+  </si>
+  <si>
+    <t>160.0</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>41.55</t>
+  </si>
+  <si>
+    <t>62.51</t>
+  </si>
+  <si>
+    <t>123.01</t>
+  </si>
+  <si>
+    <t>39.90</t>
+  </si>
+  <si>
+    <t>61.32</t>
+  </si>
+  <si>
+    <t>122.29</t>
+  </si>
+  <si>
+    <t>185.0</t>
+  </si>
+  <si>
+    <t>41.11</t>
+  </si>
+  <si>
+    <t>61.85</t>
+  </si>
+  <si>
+    <t>122.97</t>
+  </si>
+  <si>
+    <t>170.0</t>
+  </si>
+  <si>
+    <t>40.51</t>
+  </si>
+  <si>
+    <t>61.67</t>
+  </si>
+  <si>
+    <t>122.69</t>
+  </si>
+  <si>
+    <t>SVR parameter:</t>
+  </si>
+  <si>
+    <t>SVR kernel:</t>
+  </si>
+  <si>
+    <t>model No</t>
+  </si>
+  <si>
+    <t>Model No</t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>poly</t>
   </si>
 </sst>
 </file>
@@ -67,12 +289,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,8 +315,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -110,7 +339,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B8FBC46-D9A0-4B37-BA88-4E06661512EC}" name="Tabelle2" displayName="Tabelle2" ref="A2:H17" totalsRowShown="0">
   <autoFilter ref="A2:H17" xr:uid="{1B8FBC46-D9A0-4B37-BA88-4E06661512EC}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{902EBFF6-079A-407F-A862-56D8C28E74CD}" name="Model Nr"/>
+    <tableColumn id="1" xr3:uid="{902EBFF6-079A-407F-A862-56D8C28E74CD}" name="Model No"/>
     <tableColumn id="2" xr3:uid="{4BF7A98C-3A48-437C-AFDA-0862EC5AAA8B}" name="Kernel"/>
     <tableColumn id="3" xr3:uid="{A0DF1711-98DA-4123-835C-A1779471B35C}" name="C"/>
     <tableColumn id="4" xr3:uid="{B754A920-3E9E-4D1E-BC94-74CA5CE3D652}" name="epsilon"/>
@@ -118,6 +347,21 @@
     <tableColumn id="6" xr3:uid="{4836F30B-D3F4-41B6-9E3B-ECFA31900F09}" name="RMSE"/>
     <tableColumn id="7" xr3:uid="{2B439724-F109-4232-9CF8-4605DC26E3B5}" name="R2"/>
     <tableColumn id="8" xr3:uid="{1ADCE4ED-CD3D-4854-BFE3-1C2D32E528A0}" name="CRPS"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A78F3FE-A3F6-45A5-8516-9068A526C336}" name="Tabelle3" displayName="Tabelle3" ref="J2:O5" totalsRowShown="0">
+  <autoFilter ref="J2:O5" xr:uid="{9A78F3FE-A3F6-45A5-8516-9068A526C336}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3591002E-845A-48E1-AFA0-24CA056D162E}" name="model No"/>
+    <tableColumn id="2" xr3:uid="{DD7A6C23-3853-4343-B91C-1A021C6408A1}" name="kernel"/>
+    <tableColumn id="3" xr3:uid="{6EB90F8F-4FCD-41C5-9920-FCEC4B2F58A9}" name="MAE"/>
+    <tableColumn id="4" xr3:uid="{40F48B3E-6ED3-4CF8-8468-1A46706C10F5}" name="RMSE"/>
+    <tableColumn id="5" xr3:uid="{656A4842-D147-48DE-AFB8-2A4D29D577C0}" name="R2"/>
+    <tableColumn id="6" xr3:uid="{D2AE4BF3-A8B5-41D4-8CAD-FF111B09B6DE}" name="CRPS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -386,128 +630,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRPS for diff kernels
</commit_message>
<xml_diff>
--- a/thesis work/code and more/models/SVR kernel and parameter scores.xlsx
+++ b/thesis work/code and more/models/SVR kernel and parameter scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Uni\Bachelorarbeit\code\BachelorThesisWPF\thesis work\code and more\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093E2739-B314-4B0B-9F95-1FA2E3760FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8703FB-04B1-42EC-A119-731A958FD8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>Kernel</t>
   </si>
@@ -274,13 +274,40 @@
   </si>
   <si>
     <t>poly</t>
+  </si>
+  <si>
+    <t>125.48</t>
+  </si>
+  <si>
+    <t>116.00</t>
+  </si>
+  <si>
+    <t>210.76</t>
+  </si>
+  <si>
+    <t>0.78</t>
+  </si>
+  <si>
+    <t>151.95</t>
+  </si>
+  <si>
+    <t>132.67</t>
+  </si>
+  <si>
+    <t>248.66</t>
+  </si>
+  <si>
+    <t>0.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 117.77</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +315,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +337,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,9 +359,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -353,15 +404,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A78F3FE-A3F6-45A5-8516-9068A526C336}" name="Tabelle3" displayName="Tabelle3" ref="J2:O5" totalsRowShown="0">
-  <autoFilter ref="J2:O5" xr:uid="{9A78F3FE-A3F6-45A5-8516-9068A526C336}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A78F3FE-A3F6-45A5-8516-9068A526C336}" name="Tabelle3" displayName="Tabelle3" ref="J2:Q5" totalsRowShown="0">
+  <autoFilter ref="J2:Q5" xr:uid="{9A78F3FE-A3F6-45A5-8516-9068A526C336}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{3591002E-845A-48E1-AFA0-24CA056D162E}" name="model No"/>
     <tableColumn id="2" xr3:uid="{DD7A6C23-3853-4343-B91C-1A021C6408A1}" name="kernel"/>
-    <tableColumn id="3" xr3:uid="{6EB90F8F-4FCD-41C5-9920-FCEC4B2F58A9}" name="MAE"/>
-    <tableColumn id="4" xr3:uid="{40F48B3E-6ED3-4CF8-8468-1A46706C10F5}" name="RMSE"/>
-    <tableColumn id="5" xr3:uid="{656A4842-D147-48DE-AFB8-2A4D29D577C0}" name="R2"/>
-    <tableColumn id="6" xr3:uid="{D2AE4BF3-A8B5-41D4-8CAD-FF111B09B6DE}" name="CRPS"/>
+    <tableColumn id="3" xr3:uid="{6EB90F8F-4FCD-41C5-9920-FCEC4B2F58A9}" name="C"/>
+    <tableColumn id="4" xr3:uid="{40F48B3E-6ED3-4CF8-8468-1A46706C10F5}" name="epsilon"/>
+    <tableColumn id="5" xr3:uid="{656A4842-D147-48DE-AFB8-2A4D29D577C0}" name="MAE"/>
+    <tableColumn id="6" xr3:uid="{D2AE4BF3-A8B5-41D4-8CAD-FF111B09B6DE}" name="RMSE"/>
+    <tableColumn id="7" xr3:uid="{78F4551F-F4A7-45C6-B475-41EEF0B7387F}" name="R2"/>
+    <tableColumn id="8" xr3:uid="{384116B8-E0FE-4029-AE2A-FE7E496502DF}" name="CRPS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -630,20 +683,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -651,7 +704,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -683,19 +736,25 @@
         <v>80</v>
       </c>
       <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
         <v>3</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>4</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>5</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -720,14 +779,32 @@
       <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>2</v>
       </c>
@@ -758,8 +835,26 @@
       <c r="K4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>3</v>
       </c>
@@ -790,8 +885,26 @@
       <c r="K5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>4</v>
       </c>
@@ -817,7 +930,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>5</v>
       </c>
@@ -843,7 +956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>6</v>
       </c>
@@ -869,7 +982,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>7</v>
       </c>
@@ -895,7 +1008,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>8</v>
       </c>
@@ -921,7 +1034,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>9</v>
       </c>
@@ -947,7 +1060,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>10</v>
       </c>
@@ -973,7 +1086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>11</v>
       </c>
@@ -999,7 +1112,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1025,7 +1138,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1051,7 +1164,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1077,7 +1190,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1104,10 +1217,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>